<commit_message>
new version more playable.
</commit_message>
<xml_diff>
--- a/mode/LoneWolf/NewEngineFormulas.xlsx
+++ b/mode/LoneWolf/NewEngineFormulas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="129">
   <si>
     <t>Truck Name</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>New Lvl</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
   </si>
 </sst>
 </file>
@@ -892,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F160" sqref="F160:F168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +930,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="7">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F2" s="6">
         <v>0</v>
@@ -948,11 +951,11 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="5">
         <f>MIN(F20:F168)</f>
-        <v>728</v>
+        <v>2600</v>
       </c>
       <c r="D4" s="5">
         <f>MAX(F20:F168)</f>
-        <v>1314</v>
+        <v>4830</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -963,7 +966,9 @@
         <v>74</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -974,7 +979,9 @@
         <v>530</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2">
+        <v>4</v>
+      </c>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1203,8 +1210,8 @@
         <v>360</v>
       </c>
       <c r="F20" s="1">
-        <f>ROUND(B20+SUM($B$20:$B$23)/4,0)</f>
-        <v>795</v>
+        <f>ROUND(B20+$C$19+$D$19*$F$6,0)+MAX(B20-$C$19,0)*2</f>
+        <v>2760</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -1222,8 +1229,8 @@
         <v>410</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" ref="F21:F23" si="0">ROUND(B21+SUM($B$20:$B$23)/4,0)</f>
-        <v>845</v>
+        <f t="shared" ref="F21:F23" si="0">ROUND(B21+$C$19+$D$19*$F$6,0)+MAX(B21-$C$19,0)*2</f>
+        <v>2910</v>
       </c>
       <c r="G21" s="1">
         <v>6</v>
@@ -1242,14 +1249,14 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>895</v>
+        <v>3060</v>
       </c>
       <c r="G22" s="1">
         <v>10</v>
       </c>
       <c r="H22" s="16">
         <f>ROUND(((F22-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1260,8 +1267,8 @@
         <v>510</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>945</v>
+        <f>ROUND(B23+$C$19+$D$19*$F$6,0)+MAX(B23-$C$19,0)*2</f>
+        <v>3210</v>
       </c>
       <c r="G23" s="1">
         <v>16</v>
@@ -1296,8 +1303,8 @@
         <v>370</v>
       </c>
       <c r="F25" s="1">
-        <f>ROUND(B25+SUM($B$25:$B$32)/8,0)</f>
-        <v>826</v>
+        <f>ROUND(B25+$C$24+$D$24*$F$6,0)+MAX(B25-$C$24,0)*2</f>
+        <v>2860</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
@@ -1315,8 +1322,8 @@
         <v>410</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" ref="F26:F32" si="2">ROUND(B26+SUM($B$25:$B$32)/8,0)</f>
-        <v>866</v>
+        <f t="shared" ref="F26:F32" si="2">ROUND(B26+$C$24+$D$24*$F$6,0)+MAX(B26-$C$24,0)*2</f>
+        <v>2980</v>
       </c>
       <c r="G26" s="1">
         <v>2</v>
@@ -1335,7 +1342,7 @@
       </c>
       <c r="F27" s="1">
         <f t="shared" si="2"/>
-        <v>891</v>
+        <v>3055</v>
       </c>
       <c r="G27" s="1">
         <v>6</v>
@@ -1354,7 +1361,7 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" si="2"/>
-        <v>906</v>
+        <v>3100</v>
       </c>
       <c r="G28" s="1">
         <v>8</v>
@@ -1373,7 +1380,7 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" si="2"/>
-        <v>916</v>
+        <v>3130</v>
       </c>
       <c r="G29" s="1">
         <v>10</v>
@@ -1392,7 +1399,7 @@
       </c>
       <c r="F30" s="1">
         <f t="shared" si="2"/>
-        <v>936</v>
+        <v>3190</v>
       </c>
       <c r="G30" s="1">
         <v>14</v>
@@ -1411,7 +1418,7 @@
       </c>
       <c r="F31" s="1">
         <f t="shared" si="2"/>
-        <v>966</v>
+        <v>3280</v>
       </c>
       <c r="G31" s="1">
         <v>16</v>
@@ -1429,8 +1436,8 @@
         <v>530</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="2"/>
-        <v>986</v>
+        <f>ROUND(B32+$C$24+$D$24*$F$6,0)+MAX(B32-$C$24,0)*2</f>
+        <v>3340</v>
       </c>
       <c r="G32" s="1">
         <v>18</v>
@@ -1465,15 +1472,15 @@
         <v>310</v>
       </c>
       <c r="F34" s="1">
-        <f>ROUND(B34+SUM($B$34:$B$41)/8,0)</f>
-        <v>728</v>
+        <f>ROUND(B34+$C$33+$D$33*$F$6,0)+MAX(B34-$C$33,0)*2</f>
+        <v>2860</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
       </c>
       <c r="H34" s="16">
         <f t="shared" ref="H34:H41" si="3">ROUND(((F34-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1484,15 +1491,15 @@
         <v>330</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" ref="F35:F41" si="4">ROUND(B35+SUM($B$34:$B$41)/8,0)</f>
-        <v>748</v>
+        <f t="shared" ref="F35:F41" si="4">ROUND(B35+$C$33+$D$33*$F$6,0)+MAX(B35-$C$33,0)*2</f>
+        <v>2920</v>
       </c>
       <c r="G35" s="1">
         <v>6</v>
       </c>
       <c r="H35" s="16">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1504,14 +1511,14 @@
       </c>
       <c r="F36" s="1">
         <f t="shared" si="4"/>
-        <v>778</v>
+        <v>3010</v>
       </c>
       <c r="G36" s="1">
         <v>8</v>
       </c>
       <c r="H36" s="16">
         <f t="shared" si="3"/>
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1523,14 +1530,14 @@
       </c>
       <c r="F37" s="1">
         <f t="shared" si="4"/>
-        <v>818</v>
+        <v>3130</v>
       </c>
       <c r="G37" s="1">
         <v>9</v>
       </c>
       <c r="H37" s="16">
         <f t="shared" si="3"/>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1542,14 +1549,14 @@
       </c>
       <c r="F38" s="1">
         <f t="shared" si="4"/>
-        <v>838</v>
+        <v>3190</v>
       </c>
       <c r="G38" s="1">
         <v>10</v>
       </c>
       <c r="H38" s="16">
         <f t="shared" si="3"/>
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1561,14 +1568,14 @@
       </c>
       <c r="F39" s="1">
         <f t="shared" si="4"/>
-        <v>878</v>
+        <v>3310</v>
       </c>
       <c r="G39" s="1">
         <v>12</v>
       </c>
       <c r="H39" s="16">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1580,14 +1587,14 @@
       </c>
       <c r="F40" s="1">
         <f t="shared" si="4"/>
-        <v>918</v>
+        <v>3430</v>
       </c>
       <c r="G40" s="1">
         <v>14</v>
       </c>
       <c r="H40" s="16">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1599,14 +1606,14 @@
       </c>
       <c r="F41" s="1">
         <f t="shared" si="4"/>
-        <v>978</v>
+        <v>3610</v>
       </c>
       <c r="G41" s="1">
         <v>16</v>
       </c>
       <c r="H41" s="16">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1634,15 +1641,15 @@
         <v>310</v>
       </c>
       <c r="F43" s="1">
-        <f>ROUND(B43+SUM($B$43:$B$49)/7,0)</f>
-        <v>729</v>
+        <f>ROUND(B43+$C$42+$D$42*$F$6,0)+MAX(B43-$C$42,0)*2</f>
+        <v>2860</v>
       </c>
       <c r="G43" s="1">
         <v>0</v>
       </c>
       <c r="H43" s="16">
         <f t="shared" ref="H43:H49" si="5">ROUND(((F43-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1653,15 +1660,15 @@
         <v>330</v>
       </c>
       <c r="F44" s="1">
-        <f t="shared" ref="F44:F49" si="6">ROUND(B44+SUM($B$43:$B$49)/7,0)</f>
-        <v>749</v>
+        <f t="shared" ref="F44:F49" si="6">ROUND(B44+$C$42+$D$42*$F$6,0)+MAX(B44-$C$42,0)*2</f>
+        <v>2920</v>
       </c>
       <c r="G44" s="1">
         <v>6</v>
       </c>
       <c r="H44" s="16">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1673,14 +1680,14 @@
       </c>
       <c r="F45" s="1">
         <f t="shared" si="6"/>
-        <v>779</v>
+        <v>3010</v>
       </c>
       <c r="G45" s="1">
         <v>8</v>
       </c>
       <c r="H45" s="16">
         <f t="shared" si="5"/>
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1692,14 +1699,14 @@
       </c>
       <c r="F46" s="1">
         <f t="shared" si="6"/>
-        <v>839</v>
+        <v>3190</v>
       </c>
       <c r="G46" s="1">
         <v>10</v>
       </c>
       <c r="H46" s="16">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1711,14 +1718,14 @@
       </c>
       <c r="F47" s="1">
         <f t="shared" si="6"/>
-        <v>869</v>
+        <v>3280</v>
       </c>
       <c r="G47" s="1">
         <v>12</v>
       </c>
       <c r="H47" s="16">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1730,14 +1737,14 @@
       </c>
       <c r="F48" s="1">
         <f t="shared" si="6"/>
-        <v>919</v>
+        <v>3430</v>
       </c>
       <c r="G48" s="1">
         <v>14</v>
       </c>
       <c r="H48" s="16">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1749,14 +1756,14 @@
       </c>
       <c r="F49" s="1">
         <f t="shared" si="6"/>
-        <v>979</v>
+        <v>3610</v>
       </c>
       <c r="G49" s="1">
         <v>16</v>
       </c>
       <c r="H49" s="16">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1784,15 +1791,15 @@
         <v>320</v>
       </c>
       <c r="F51" s="1">
-        <f>ROUND(B51+SUM($B$51:$B$57)/7,0)</f>
-        <v>780</v>
+        <f>ROUND(B51+$C$50+$D$50*$F$6,0)+MAX(B51-$C$50,0)*2</f>
+        <v>3360</v>
       </c>
       <c r="G51" s="1">
         <v>0</v>
       </c>
       <c r="H51" s="16">
         <f t="shared" ref="H51:H57" si="7">ROUND(((F51-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1803,15 +1810,15 @@
         <v>360</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" ref="F52:F57" si="8">ROUND(B52+SUM($B$51:$B$57)/7,0)</f>
-        <v>820</v>
+        <f t="shared" ref="F52:F57" si="8">ROUND(B52+$C$50+$D$50*$F$6,0)+MAX(B52-$C$50,0)*2</f>
+        <v>3480</v>
       </c>
       <c r="G52" s="1">
         <v>6</v>
       </c>
       <c r="H52" s="16">
         <f t="shared" si="7"/>
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1823,14 +1830,14 @@
       </c>
       <c r="F53" s="1">
         <f t="shared" si="8"/>
-        <v>860</v>
+        <v>3600</v>
       </c>
       <c r="G53" s="1">
         <v>8</v>
       </c>
       <c r="H53" s="16">
         <f t="shared" si="7"/>
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1842,14 +1849,14 @@
       </c>
       <c r="F54" s="1">
         <f t="shared" si="8"/>
-        <v>900</v>
+        <v>3720</v>
       </c>
       <c r="G54" s="1">
         <v>10</v>
       </c>
       <c r="H54" s="16">
         <f t="shared" si="7"/>
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1861,14 +1868,14 @@
       </c>
       <c r="F55" s="1">
         <f t="shared" si="8"/>
-        <v>940</v>
+        <v>3840</v>
       </c>
       <c r="G55" s="1">
         <v>12</v>
       </c>
       <c r="H55" s="16">
         <f t="shared" si="7"/>
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1880,14 +1887,14 @@
       </c>
       <c r="F56" s="1">
         <f t="shared" si="8"/>
-        <v>1000</v>
+        <v>4020</v>
       </c>
       <c r="G56" s="1">
         <v>14</v>
       </c>
       <c r="H56" s="16">
         <f t="shared" si="7"/>
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1899,14 +1906,14 @@
       </c>
       <c r="F57" s="1">
         <f t="shared" si="8"/>
-        <v>1140</v>
+        <v>4440</v>
       </c>
       <c r="G57" s="1">
         <v>16</v>
       </c>
       <c r="H57" s="16">
         <f t="shared" si="7"/>
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1934,15 +1941,15 @@
         <v>360</v>
       </c>
       <c r="F59" s="1">
-        <f>ROUND(B59+SUM($B$59:$B$65)/7,0)</f>
-        <v>846</v>
+        <f>ROUND(B59+$C$58+$D$58*$F$6,0)+MAX(B59-$C$58,0)*2</f>
+        <v>3280</v>
       </c>
       <c r="G59" s="1">
         <v>0</v>
       </c>
       <c r="H59" s="16">
         <f t="shared" ref="H59:H65" si="9">ROUND(((F59-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1953,15 +1960,15 @@
         <v>400</v>
       </c>
       <c r="F60" s="1">
-        <f t="shared" ref="F60:F65" si="10">ROUND(B60+SUM($B$59:$B$65)/7,0)</f>
-        <v>886</v>
+        <f t="shared" ref="F60:F65" si="10">ROUND(B60+$C$58+$D$58*$F$6,0)+MAX(B60-$C$58,0)*2</f>
+        <v>3400</v>
       </c>
       <c r="G60" s="1">
         <v>6</v>
       </c>
       <c r="H60" s="16">
         <f t="shared" si="9"/>
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1973,14 +1980,14 @@
       </c>
       <c r="F61" s="1">
         <f t="shared" si="10"/>
-        <v>926</v>
+        <v>3520</v>
       </c>
       <c r="G61" s="1">
         <v>8</v>
       </c>
       <c r="H61" s="16">
         <f t="shared" si="9"/>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1992,14 +1999,14 @@
       </c>
       <c r="F62" s="1">
         <f t="shared" si="10"/>
-        <v>966</v>
+        <v>3640</v>
       </c>
       <c r="G62" s="1">
         <v>12</v>
       </c>
       <c r="H62" s="16">
         <f t="shared" si="9"/>
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2011,14 +2018,14 @@
       </c>
       <c r="F63" s="1">
         <f t="shared" si="10"/>
-        <v>1006</v>
+        <v>3760</v>
       </c>
       <c r="G63" s="1">
         <v>16</v>
       </c>
       <c r="H63" s="16">
         <f t="shared" si="9"/>
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2030,14 +2037,14 @@
       </c>
       <c r="F64" s="1">
         <f t="shared" si="10"/>
-        <v>1046</v>
+        <v>3880</v>
       </c>
       <c r="G64" s="1">
         <v>18</v>
       </c>
       <c r="H64" s="16">
         <f t="shared" si="9"/>
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2049,14 +2056,14 @@
       </c>
       <c r="F65" s="1">
         <f t="shared" si="10"/>
-        <v>1126</v>
+        <v>4120</v>
       </c>
       <c r="G65" s="1">
         <v>20</v>
       </c>
       <c r="H65" s="16">
         <f t="shared" si="9"/>
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2084,15 +2091,15 @@
         <v>320</v>
       </c>
       <c r="F67" s="1">
-        <f>ROUND(B67+SUM($B$67:$B$75)/9,0)</f>
-        <v>777</v>
+        <f>ROUND(B67+$C$66+$D$66*$F$6,0)+MAX(B67-$C$66,0)*2</f>
+        <v>3032</v>
       </c>
       <c r="G67" s="1">
         <v>0</v>
       </c>
       <c r="H67" s="16">
         <f t="shared" ref="H67:H75" si="11">ROUND(((F67-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2103,15 +2110,15 @@
         <v>360</v>
       </c>
       <c r="F68" s="1">
-        <f t="shared" ref="F68:F75" si="12">ROUND(B68+SUM($B$67:$B$75)/9,0)</f>
-        <v>817</v>
+        <f t="shared" ref="F68:F75" si="12">ROUND(B68+$C$66+$D$66*$F$6,0)+MAX(B68-$C$66,0)*2</f>
+        <v>3152</v>
       </c>
       <c r="G68" s="1">
         <v>6</v>
       </c>
       <c r="H68" s="16">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2123,14 +2130,14 @@
       </c>
       <c r="F69" s="1">
         <f t="shared" si="12"/>
-        <v>865</v>
+        <v>3296</v>
       </c>
       <c r="G69" s="1">
         <v>8</v>
       </c>
       <c r="H69" s="16">
         <f t="shared" si="11"/>
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2142,14 +2149,14 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" si="12"/>
-        <v>892</v>
+        <v>3377</v>
       </c>
       <c r="G70" s="1">
         <v>10</v>
       </c>
       <c r="H70" s="16">
         <f t="shared" si="11"/>
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2161,14 +2168,14 @@
       </c>
       <c r="F71" s="1">
         <f t="shared" si="12"/>
-        <v>913</v>
+        <v>3440</v>
       </c>
       <c r="G71" s="1">
         <v>12</v>
       </c>
       <c r="H71" s="16">
         <f t="shared" si="11"/>
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2180,14 +2187,14 @@
       </c>
       <c r="F72" s="1">
         <f t="shared" si="12"/>
-        <v>933</v>
+        <v>3500</v>
       </c>
       <c r="G72" s="1">
         <v>14</v>
       </c>
       <c r="H72" s="16">
         <f t="shared" si="11"/>
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2199,14 +2206,14 @@
       </c>
       <c r="F73" s="1">
         <f t="shared" si="12"/>
-        <v>967</v>
+        <v>3602</v>
       </c>
       <c r="G73" s="1">
         <v>16</v>
       </c>
       <c r="H73" s="16">
         <f t="shared" si="11"/>
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2218,14 +2225,14 @@
       </c>
       <c r="F74" s="1">
         <f t="shared" si="12"/>
-        <v>1008</v>
+        <v>3725</v>
       </c>
       <c r="G74" s="1">
         <v>18</v>
       </c>
       <c r="H74" s="16">
         <f t="shared" si="11"/>
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2237,14 +2244,14 @@
       </c>
       <c r="F75" s="1">
         <f t="shared" si="12"/>
-        <v>1055</v>
+        <v>3866</v>
       </c>
       <c r="G75" s="1">
         <v>20</v>
       </c>
       <c r="H75" s="16">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2272,15 +2279,15 @@
         <v>421</v>
       </c>
       <c r="F77" s="1">
-        <f>ROUND(B77+SUM($B$77:$B$83)/7,0)</f>
-        <v>932</v>
+        <f>ROUND(B77+$C$76+$D$76*$F$6,0)+MAX(B77-$C$76,0)*2</f>
+        <v>3342</v>
       </c>
       <c r="G77" s="1">
         <v>0</v>
       </c>
       <c r="H77" s="16">
         <f t="shared" ref="H77:H83" si="13">ROUND(((F77-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2291,15 +2298,15 @@
         <v>449</v>
       </c>
       <c r="F78" s="1">
-        <f t="shared" ref="F78:F83" si="14">ROUND(B78+SUM($B$77:$B$83)/7,0)</f>
-        <v>960</v>
+        <f t="shared" ref="F78:F83" si="14">ROUND(B78+$C$76+$D$76*$F$6,0)+MAX(B78-$C$76,0)*2</f>
+        <v>3426</v>
       </c>
       <c r="G78" s="1">
         <v>6</v>
       </c>
       <c r="H78" s="16">
         <f t="shared" si="13"/>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2311,14 +2318,14 @@
       </c>
       <c r="F79" s="1">
         <f t="shared" si="14"/>
-        <v>987</v>
+        <v>3507</v>
       </c>
       <c r="G79" s="1">
         <v>10</v>
       </c>
       <c r="H79" s="16">
         <f t="shared" si="13"/>
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2330,14 +2337,14 @@
       </c>
       <c r="F80" s="1">
         <f t="shared" si="14"/>
-        <v>1021</v>
+        <v>3609</v>
       </c>
       <c r="G80" s="1">
         <v>12</v>
       </c>
       <c r="H80" s="16">
         <f t="shared" si="13"/>
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2349,14 +2356,14 @@
       </c>
       <c r="F81" s="1">
         <f t="shared" si="14"/>
-        <v>1028</v>
+        <v>3630</v>
       </c>
       <c r="G81" s="1">
         <v>14</v>
       </c>
       <c r="H81" s="16">
         <f t="shared" si="13"/>
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2368,14 +2375,14 @@
       </c>
       <c r="F82" s="1">
         <f t="shared" si="14"/>
-        <v>1089</v>
+        <v>3813</v>
       </c>
       <c r="G82" s="1">
         <v>16</v>
       </c>
       <c r="H82" s="16">
         <f t="shared" si="13"/>
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2387,14 +2394,14 @@
       </c>
       <c r="F83" s="1">
         <f t="shared" si="14"/>
-        <v>1136</v>
+        <v>3954</v>
       </c>
       <c r="G83" s="1">
         <v>20</v>
       </c>
       <c r="H83" s="16">
         <f t="shared" si="13"/>
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -2422,15 +2429,15 @@
         <v>440</v>
       </c>
       <c r="F85" s="1">
-        <f>ROUND(B85+SUM($B$85:$B$87)/3,0)</f>
-        <v>920</v>
+        <f>ROUND(B85+$C$84+$D$84*$F$6,0)+MAX(B85-$C$84,0)*2</f>
+        <v>2960</v>
       </c>
       <c r="G85" s="1">
         <v>0</v>
       </c>
       <c r="H85" s="16">
         <f>ROUND(((F85-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2441,15 +2448,15 @@
         <v>480</v>
       </c>
       <c r="F86" s="1">
-        <f t="shared" ref="F86:F87" si="15">ROUND(B86+SUM($B$85:$B$87)/3,0)</f>
-        <v>960</v>
+        <f t="shared" ref="F86:F87" si="15">ROUND(B86+$C$84+$D$84*$F$6,0)+MAX(B86-$C$84,0)*2</f>
+        <v>3080</v>
       </c>
       <c r="G86" s="1">
         <v>10</v>
       </c>
       <c r="H86" s="16">
         <f>ROUND(((F86-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="87" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2461,14 +2468,14 @@
       </c>
       <c r="F87" s="1">
         <f t="shared" si="15"/>
-        <v>1000</v>
+        <v>3200</v>
       </c>
       <c r="G87" s="1">
         <v>16</v>
       </c>
       <c r="H87" s="16">
         <f>ROUND(((F87-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -2496,15 +2503,15 @@
         <v>380</v>
       </c>
       <c r="F89" s="1">
-        <f>ROUND(B89+SUM($B$89:$B$91)/3,0)</f>
-        <v>803</v>
+        <f>ROUND(B89+$C$88+$D$88*$F$6,0)+MAX(B89-$C$88,0)*2</f>
+        <v>2600</v>
       </c>
       <c r="G89" s="1">
         <v>0</v>
       </c>
       <c r="H89" s="16">
         <f>ROUND(((F89-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2515,15 +2522,15 @@
         <v>430</v>
       </c>
       <c r="F90" s="1">
-        <f t="shared" ref="F90:F91" si="16">ROUND(B90+SUM($B$89:$B$91)/3,0)</f>
-        <v>853</v>
+        <f t="shared" ref="F90:F91" si="16">ROUND(B90+$C$88+$D$88*$F$6,0)+MAX(B90-$C$88,0)*2</f>
+        <v>2750</v>
       </c>
       <c r="G90" s="1">
         <v>10</v>
       </c>
       <c r="H90" s="16">
         <f>ROUND(((F90-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2535,14 +2542,14 @@
       </c>
       <c r="F91" s="1">
         <f t="shared" si="16"/>
-        <v>883</v>
+        <v>2840</v>
       </c>
       <c r="G91" s="1">
         <v>16</v>
       </c>
       <c r="H91" s="16">
         <f>ROUND(((F91-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -2570,15 +2577,15 @@
         <v>380</v>
       </c>
       <c r="F93" s="1">
-        <f>ROUND(B93+SUM($B$93:$B$98)/6,0)</f>
-        <v>832</v>
+        <f>ROUND(B93+$C$92+$D$92*$F$6,0)+MAX(B93-$C$92,0)*2</f>
+        <v>2840</v>
       </c>
       <c r="G93" s="1">
         <v>0</v>
       </c>
       <c r="H93" s="16">
         <f t="shared" ref="H93:H98" si="17">ROUND(((F93-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2589,15 +2596,15 @@
         <v>430</v>
       </c>
       <c r="F94" s="1">
-        <f t="shared" ref="F94:F98" si="18">ROUND(B94+SUM($B$93:$B$98)/6,0)</f>
-        <v>882</v>
+        <f t="shared" ref="F94:F98" si="18">ROUND(B94+$C$92+$D$92*$F$6,0)+MAX(B94-$C$92,0)*2</f>
+        <v>2990</v>
       </c>
       <c r="G94" s="1">
         <v>10</v>
       </c>
       <c r="H94" s="16">
         <f t="shared" si="17"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2609,7 +2616,7 @@
       </c>
       <c r="F95" s="1">
         <f t="shared" si="18"/>
-        <v>892</v>
+        <v>3020</v>
       </c>
       <c r="G95" s="1">
         <v>12</v>
@@ -2628,7 +2635,7 @@
       </c>
       <c r="F96" s="1">
         <f t="shared" si="18"/>
-        <v>912</v>
+        <v>3080</v>
       </c>
       <c r="G96" s="1">
         <v>14</v>
@@ -2647,7 +2654,7 @@
       </c>
       <c r="F97" s="1">
         <f t="shared" si="18"/>
-        <v>932</v>
+        <v>3140</v>
       </c>
       <c r="G97" s="1">
         <v>16</v>
@@ -2666,7 +2673,7 @@
       </c>
       <c r="F98" s="1">
         <f t="shared" si="18"/>
-        <v>972</v>
+        <v>3260</v>
       </c>
       <c r="G98" s="1">
         <v>18</v>
@@ -2701,15 +2708,15 @@
         <v>360</v>
       </c>
       <c r="F100" s="1">
-        <f>ROUND(B100+SUM($B$100:$B$111)/12,0)</f>
-        <v>844</v>
+        <f>ROUND(B100+$C$99+$D$99*$F$6,0)+MAX(B100-$C$99,0)*2</f>
+        <v>3640</v>
       </c>
       <c r="G100" s="1">
         <v>0</v>
       </c>
       <c r="H100" s="16">
         <f t="shared" ref="H100:H111" si="19">ROUND(((F100-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="101" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2720,15 +2727,15 @@
         <v>380</v>
       </c>
       <c r="F101" s="1">
-        <f t="shared" ref="F101:F111" si="20">ROUND(B101+SUM($B$100:$B$111)/12,0)</f>
-        <v>864</v>
+        <f t="shared" ref="F101:F111" si="20">ROUND(B101+$C$99+$D$99*$F$6,0)+MAX(B101-$C$99,0)*2</f>
+        <v>3700</v>
       </c>
       <c r="G101" s="1">
         <v>8</v>
       </c>
       <c r="H101" s="16">
         <f t="shared" si="19"/>
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2740,14 +2747,14 @@
       </c>
       <c r="F102" s="1">
         <f t="shared" si="20"/>
-        <v>884</v>
+        <v>3760</v>
       </c>
       <c r="G102" s="1">
         <v>8</v>
       </c>
       <c r="H102" s="16">
         <f t="shared" si="19"/>
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="103" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2759,14 +2766,14 @@
       </c>
       <c r="F103" s="1">
         <f t="shared" si="20"/>
-        <v>904</v>
+        <v>3820</v>
       </c>
       <c r="G103" s="1">
         <v>10</v>
       </c>
       <c r="H103" s="16">
         <f t="shared" si="19"/>
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2778,14 +2785,14 @@
       </c>
       <c r="F104" s="1">
         <f t="shared" si="20"/>
-        <v>924</v>
+        <v>3880</v>
       </c>
       <c r="G104" s="1">
         <v>12</v>
       </c>
       <c r="H104" s="16">
         <f t="shared" si="19"/>
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="105" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2797,14 +2804,14 @@
       </c>
       <c r="F105" s="1">
         <f t="shared" si="20"/>
-        <v>924</v>
+        <v>3880</v>
       </c>
       <c r="G105" s="1">
         <v>12</v>
       </c>
       <c r="H105" s="16">
         <f t="shared" si="19"/>
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2816,14 +2823,14 @@
       </c>
       <c r="F106" s="1">
         <f t="shared" si="20"/>
-        <v>964</v>
+        <v>4000</v>
       </c>
       <c r="G106" s="1">
         <v>14</v>
       </c>
       <c r="H106" s="16">
         <f t="shared" si="19"/>
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="107" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2835,14 +2842,14 @@
       </c>
       <c r="F107" s="1">
         <f t="shared" si="20"/>
-        <v>964</v>
+        <v>4000</v>
       </c>
       <c r="G107" s="1">
         <v>14</v>
       </c>
       <c r="H107" s="16">
         <f t="shared" si="19"/>
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="108" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2854,14 +2861,14 @@
       </c>
       <c r="F108" s="1">
         <f t="shared" si="20"/>
-        <v>984</v>
+        <v>4060</v>
       </c>
       <c r="G108" s="1">
         <v>16</v>
       </c>
       <c r="H108" s="16">
         <f t="shared" si="19"/>
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="109" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2873,14 +2880,14 @@
       </c>
       <c r="F109" s="1">
         <f t="shared" si="20"/>
-        <v>1044</v>
+        <v>4240</v>
       </c>
       <c r="G109" s="1">
         <v>18</v>
       </c>
       <c r="H109" s="16">
         <f t="shared" si="19"/>
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="110" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2892,14 +2899,14 @@
       </c>
       <c r="F110" s="1">
         <f t="shared" si="20"/>
-        <v>1104</v>
+        <v>4420</v>
       </c>
       <c r="G110" s="1">
         <v>20</v>
       </c>
       <c r="H110" s="16">
         <f t="shared" si="19"/>
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="111" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2911,14 +2918,14 @@
       </c>
       <c r="F111" s="1">
         <f t="shared" si="20"/>
-        <v>1214</v>
+        <v>4750</v>
       </c>
       <c r="G111" s="1">
         <v>25</v>
       </c>
       <c r="H111" s="16">
         <f t="shared" si="19"/>
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -2946,15 +2953,15 @@
         <v>370</v>
       </c>
       <c r="F113" s="1">
-        <f>ROUND(B113+SUM($B$113:$B$120)/8,0)</f>
-        <v>896</v>
+        <f>ROUND(B113+$C$112+$D$112*$F$6,0)+MAX(B113-$C$112,0)*2</f>
+        <v>3660</v>
       </c>
       <c r="G113" s="1">
         <v>0</v>
       </c>
       <c r="H113" s="16">
         <f t="shared" ref="H113:H120" si="21">ROUND(((F113-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2965,15 +2972,15 @@
         <v>410</v>
       </c>
       <c r="F114" s="1">
-        <f t="shared" ref="F114:F120" si="22">ROUND(B114+SUM($B$113:$B$120)/8,0)</f>
-        <v>936</v>
+        <f t="shared" ref="F114:F120" si="22">ROUND(B114+$C$112+$D$112*$F$6,0)+MAX(B114-$C$112,0)*2</f>
+        <v>3780</v>
       </c>
       <c r="G114" s="1">
         <v>6</v>
       </c>
       <c r="H114" s="16">
         <f t="shared" si="21"/>
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2985,14 +2992,14 @@
       </c>
       <c r="F115" s="1">
         <f t="shared" si="22"/>
-        <v>976</v>
+        <v>3900</v>
       </c>
       <c r="G115" s="1">
         <v>10</v>
       </c>
       <c r="H115" s="16">
         <f t="shared" si="21"/>
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3004,14 +3011,14 @@
       </c>
       <c r="F116" s="1">
         <f t="shared" si="22"/>
-        <v>1026</v>
+        <v>4050</v>
       </c>
       <c r="G116" s="1">
         <v>12</v>
       </c>
       <c r="H116" s="16">
         <f t="shared" si="21"/>
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3023,14 +3030,14 @@
       </c>
       <c r="F117" s="1">
         <f t="shared" si="22"/>
-        <v>1046</v>
+        <v>4110</v>
       </c>
       <c r="G117" s="1">
         <v>15</v>
       </c>
       <c r="H117" s="16">
         <f t="shared" si="21"/>
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="118" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3042,14 +3049,14 @@
       </c>
       <c r="F118" s="1">
         <f t="shared" si="22"/>
-        <v>1106</v>
+        <v>4290</v>
       </c>
       <c r="G118" s="1">
         <v>18</v>
       </c>
       <c r="H118" s="16">
         <f t="shared" si="21"/>
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3061,14 +3068,14 @@
       </c>
       <c r="F119" s="1">
         <f t="shared" si="22"/>
-        <v>1176</v>
+        <v>4500</v>
       </c>
       <c r="G119" s="1">
         <v>20</v>
       </c>
       <c r="H119" s="16">
         <f t="shared" si="21"/>
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="120" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3080,14 +3087,14 @@
       </c>
       <c r="F120" s="1">
         <f t="shared" si="22"/>
-        <v>1256</v>
+        <v>4740</v>
       </c>
       <c r="G120" s="1">
         <v>25</v>
       </c>
       <c r="H120" s="16">
         <f t="shared" si="21"/>
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -3115,15 +3122,15 @@
         <v>370</v>
       </c>
       <c r="F122" s="1">
-        <f>ROUND(B122+SUM($B$122:$B$129)/8,0)</f>
-        <v>896</v>
+        <f>ROUND(B122+$C$121+$D$121*$F$6,0)+MAX(B122-$C$121,0)*2</f>
+        <v>3660</v>
       </c>
       <c r="G122" s="1">
         <v>0</v>
       </c>
       <c r="H122" s="16">
         <f t="shared" ref="H122:H129" si="23">ROUND(((F122-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3134,15 +3141,15 @@
         <v>410</v>
       </c>
       <c r="F123" s="1">
-        <f t="shared" ref="F123:F129" si="24">ROUND(B123+SUM($B$122:$B$129)/8,0)</f>
-        <v>936</v>
+        <f t="shared" ref="F123:F129" si="24">ROUND(B123+$C$121+$D$121*$F$6,0)+MAX(B123-$C$121,0)*2</f>
+        <v>3780</v>
       </c>
       <c r="G123" s="1">
         <v>6</v>
       </c>
       <c r="H123" s="16">
         <f t="shared" si="23"/>
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="124" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3154,14 +3161,14 @@
       </c>
       <c r="F124" s="1">
         <f t="shared" si="24"/>
-        <v>976</v>
+        <v>3900</v>
       </c>
       <c r="G124" s="1">
         <v>10</v>
       </c>
       <c r="H124" s="16">
         <f t="shared" si="23"/>
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="125" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3173,14 +3180,14 @@
       </c>
       <c r="F125" s="1">
         <f t="shared" si="24"/>
-        <v>1026</v>
+        <v>4050</v>
       </c>
       <c r="G125" s="1">
         <v>12</v>
       </c>
       <c r="H125" s="16">
         <f t="shared" si="23"/>
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="126" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3192,14 +3199,14 @@
       </c>
       <c r="F126" s="1">
         <f t="shared" si="24"/>
-        <v>1046</v>
+        <v>4110</v>
       </c>
       <c r="G126" s="1">
         <v>15</v>
       </c>
       <c r="H126" s="16">
         <f t="shared" si="23"/>
-        <v>26</v>
+        <v>37</v>
       </c>
     </row>
     <row r="127" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3211,14 +3218,14 @@
       </c>
       <c r="F127" s="1">
         <f t="shared" si="24"/>
-        <v>1106</v>
+        <v>4290</v>
       </c>
       <c r="G127" s="1">
         <v>18</v>
       </c>
       <c r="H127" s="16">
         <f t="shared" si="23"/>
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="128" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3230,14 +3237,14 @@
       </c>
       <c r="F128" s="1">
         <f t="shared" si="24"/>
-        <v>1176</v>
+        <v>4500</v>
       </c>
       <c r="G128" s="1">
         <v>20</v>
       </c>
       <c r="H128" s="16">
         <f t="shared" si="23"/>
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="129" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3249,14 +3256,14 @@
       </c>
       <c r="F129" s="1">
         <f t="shared" si="24"/>
-        <v>1256</v>
+        <v>4740</v>
       </c>
       <c r="G129" s="1">
         <v>25</v>
       </c>
       <c r="H129" s="16">
         <f t="shared" si="23"/>
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -3284,15 +3291,15 @@
         <v>360</v>
       </c>
       <c r="F131" s="1">
-        <f>ROUND(B131+SUM($B$131:$B$149)/19,0)</f>
-        <v>853</v>
+        <f>ROUND(B131+$C$130+$D$130*$F$6,0)+MAX(B131-$C$130,0)*2</f>
+        <v>3640</v>
       </c>
       <c r="G131" s="1">
         <v>0</v>
       </c>
       <c r="H131" s="16">
         <f t="shared" ref="H131:H154" si="25">ROUND(((F131-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="132" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3303,15 +3310,15 @@
         <v>370</v>
       </c>
       <c r="F132" s="1">
-        <f t="shared" ref="F132:F149" si="26">ROUND(B132+SUM($B$131:$B$149)/19,0)</f>
-        <v>863</v>
+        <f t="shared" ref="F132:F149" si="26">ROUND(B132+$C$130+$D$130*$F$6,0)+MAX(B132-$C$130,0)*2</f>
+        <v>3670</v>
       </c>
       <c r="G132" s="1">
         <v>3</v>
       </c>
       <c r="H132" s="16">
         <f t="shared" si="25"/>
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="133" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3323,14 +3330,14 @@
       </c>
       <c r="F133" s="1">
         <f t="shared" si="26"/>
-        <v>873</v>
+        <v>3700</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
       </c>
       <c r="H133" s="16">
         <f t="shared" si="25"/>
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="134" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3342,14 +3349,14 @@
       </c>
       <c r="F134" s="1">
         <f t="shared" si="26"/>
-        <v>893</v>
+        <v>3760</v>
       </c>
       <c r="G134" s="1">
         <v>8</v>
       </c>
       <c r="H134" s="16">
         <f t="shared" si="25"/>
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="135" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3361,14 +3368,14 @@
       </c>
       <c r="F135" s="1">
         <f t="shared" si="26"/>
-        <v>903</v>
+        <v>3790</v>
       </c>
       <c r="G135" s="1">
         <v>12</v>
       </c>
       <c r="H135" s="16">
         <f t="shared" si="25"/>
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="136" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3380,14 +3387,14 @@
       </c>
       <c r="F136" s="1">
         <f t="shared" si="26"/>
-        <v>913</v>
+        <v>3820</v>
       </c>
       <c r="G136" s="1">
         <v>10</v>
       </c>
       <c r="H136" s="16">
         <f t="shared" si="25"/>
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="137" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3399,14 +3406,14 @@
       </c>
       <c r="F137" s="1">
         <f t="shared" si="26"/>
-        <v>933</v>
+        <v>3880</v>
       </c>
       <c r="G137" s="1">
         <v>12</v>
       </c>
       <c r="H137" s="16">
         <f t="shared" si="25"/>
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3418,14 +3425,14 @@
       </c>
       <c r="F138" s="1">
         <f t="shared" si="26"/>
-        <v>933</v>
+        <v>3880</v>
       </c>
       <c r="G138" s="1">
         <v>12</v>
       </c>
       <c r="H138" s="16">
         <f t="shared" si="25"/>
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3437,14 +3444,14 @@
       </c>
       <c r="F139" s="1">
         <f t="shared" si="26"/>
-        <v>943</v>
+        <v>3910</v>
       </c>
       <c r="G139" s="1">
         <v>14</v>
       </c>
       <c r="H139" s="16">
         <f t="shared" si="25"/>
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3456,14 +3463,14 @@
       </c>
       <c r="F140" s="1">
         <f t="shared" si="26"/>
-        <v>973</v>
+        <v>4000</v>
       </c>
       <c r="G140" s="1">
         <v>14</v>
       </c>
       <c r="H140" s="16">
         <f t="shared" si="25"/>
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="141" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3475,14 +3482,14 @@
       </c>
       <c r="F141" s="1">
         <f t="shared" si="26"/>
-        <v>973</v>
+        <v>4000</v>
       </c>
       <c r="G141" s="1">
         <v>14</v>
       </c>
       <c r="H141" s="16">
         <f t="shared" si="25"/>
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="142" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3494,14 +3501,14 @@
       </c>
       <c r="F142" s="1">
         <f t="shared" si="26"/>
-        <v>983</v>
+        <v>4030</v>
       </c>
       <c r="G142" s="1">
         <v>15</v>
       </c>
       <c r="H142" s="16">
         <f t="shared" si="25"/>
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="143" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3513,14 +3520,14 @@
       </c>
       <c r="F143" s="1">
         <f t="shared" si="26"/>
-        <v>993</v>
+        <v>4060</v>
       </c>
       <c r="G143" s="1">
         <v>16</v>
       </c>
       <c r="H143" s="16">
         <f t="shared" si="25"/>
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="144" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3532,14 +3539,14 @@
       </c>
       <c r="F144" s="1">
         <f t="shared" si="26"/>
-        <v>1013</v>
+        <v>4120</v>
       </c>
       <c r="G144" s="1">
         <v>17</v>
       </c>
       <c r="H144" s="16">
         <f t="shared" si="25"/>
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="145" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3551,14 +3558,14 @@
       </c>
       <c r="F145" s="1">
         <f t="shared" si="26"/>
-        <v>1053</v>
+        <v>4240</v>
       </c>
       <c r="G145" s="1">
         <v>18</v>
       </c>
       <c r="H145" s="16">
         <f t="shared" si="25"/>
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="146" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3570,14 +3577,14 @@
       </c>
       <c r="F146" s="1">
         <f t="shared" si="26"/>
-        <v>1073</v>
+        <v>4300</v>
       </c>
       <c r="G146" s="1">
         <v>18</v>
       </c>
       <c r="H146" s="16">
         <f t="shared" si="25"/>
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="147" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3589,14 +3596,14 @@
       </c>
       <c r="F147" s="1">
         <f t="shared" si="26"/>
-        <v>1113</v>
+        <v>4420</v>
       </c>
       <c r="G147" s="1">
         <v>20</v>
       </c>
       <c r="H147" s="16">
         <f t="shared" si="25"/>
-        <v>30</v>
+        <v>43</v>
       </c>
     </row>
     <row r="148" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3608,14 +3615,14 @@
       </c>
       <c r="F148" s="1">
         <f t="shared" si="26"/>
-        <v>1223</v>
+        <v>4750</v>
       </c>
       <c r="G148" s="1">
         <v>24</v>
       </c>
       <c r="H148" s="16">
         <f t="shared" si="25"/>
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="149" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3627,14 +3634,14 @@
       </c>
       <c r="F149" s="1">
         <f t="shared" si="26"/>
-        <v>1223</v>
+        <v>4750</v>
       </c>
       <c r="G149" s="1">
         <v>25</v>
       </c>
       <c r="H149" s="16">
         <f t="shared" si="25"/>
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -3643,7 +3650,7 @@
       </c>
       <c r="B150" s="5"/>
       <c r="C150" s="5">
-        <v>540</v>
+        <v>420</v>
       </c>
       <c r="D150" s="5">
         <v>750</v>
@@ -3662,15 +3669,15 @@
         <v>420</v>
       </c>
       <c r="F151" s="1">
-        <f>ROUND(B151+SUM($B$151:$B$158)/8,0)</f>
-        <v>984</v>
+        <f>ROUND(B151+$C$150+$D$150*$F$6,0)+MAX(B151-$C$150,0)*2</f>
+        <v>3840</v>
       </c>
       <c r="G151" s="1">
         <v>0</v>
       </c>
       <c r="H151" s="16">
         <f t="shared" si="25"/>
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="152" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3681,15 +3688,15 @@
         <v>460</v>
       </c>
       <c r="F152" s="1">
-        <f t="shared" ref="F152:F158" si="27">ROUND(B152+SUM($B$151:$B$158)/8,0)</f>
-        <v>1024</v>
+        <f t="shared" ref="F152:F158" si="27">ROUND(B152+$C$150+$D$150*$F$6,0)+MAX(B152-$C$150,0)*2</f>
+        <v>3960</v>
       </c>
       <c r="G152" s="1">
         <v>2</v>
       </c>
       <c r="H152" s="16">
         <f t="shared" si="25"/>
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="153" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3701,14 +3708,14 @@
       </c>
       <c r="F153" s="1">
         <f t="shared" si="27"/>
-        <v>1064</v>
+        <v>4080</v>
       </c>
       <c r="G153" s="1">
         <v>6</v>
       </c>
       <c r="H153" s="16">
         <f t="shared" si="25"/>
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="154" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3720,14 +3727,14 @@
       </c>
       <c r="F154" s="1">
         <f t="shared" si="27"/>
-        <v>1104</v>
+        <v>4200</v>
       </c>
       <c r="G154" s="1">
         <v>11</v>
       </c>
       <c r="H154" s="16">
         <f t="shared" si="25"/>
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="155" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3739,14 +3746,14 @@
       </c>
       <c r="F155" s="1">
         <f t="shared" si="27"/>
-        <v>1104</v>
+        <v>4200</v>
       </c>
       <c r="G155" s="1">
         <v>0</v>
       </c>
       <c r="H155" s="16">
         <f>ROUND(((F155-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="156" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3758,14 +3765,14 @@
       </c>
       <c r="F156" s="1">
         <f t="shared" si="27"/>
-        <v>1164</v>
+        <v>4380</v>
       </c>
       <c r="G156" s="1">
         <v>6</v>
       </c>
       <c r="H156" s="16">
         <f>ROUND(((F156-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="157" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3777,14 +3784,14 @@
       </c>
       <c r="F157" s="1">
         <f t="shared" si="27"/>
-        <v>1264</v>
+        <v>4680</v>
       </c>
       <c r="G157" s="1">
         <v>10</v>
       </c>
       <c r="H157" s="16">
         <f>ROUND(((F157-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="158" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3796,14 +3803,14 @@
       </c>
       <c r="F158" s="1">
         <f t="shared" si="27"/>
-        <v>1314</v>
+        <v>4830</v>
       </c>
       <c r="G158" s="1">
         <v>16</v>
       </c>
       <c r="H158" s="16">
         <f>ROUND(((F158-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -3831,15 +3838,15 @@
         <v>420</v>
       </c>
       <c r="F160" s="1">
-        <f>ROUND(B160+SUM($B$160:$B$168)/9,0)</f>
-        <v>972</v>
+        <f>ROUND(B160+$C$159+$D$159*$F$6,0)+MAX(B160-$C$159,0)*2</f>
+        <v>3840</v>
       </c>
       <c r="G160" s="1">
         <v>0</v>
       </c>
       <c r="H160" s="16">
         <f t="shared" ref="H160:H168" si="28">ROUND(((F160-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="161" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3850,15 +3857,15 @@
         <v>460</v>
       </c>
       <c r="F161" s="1">
-        <f t="shared" ref="F161:F168" si="29">ROUND(B161+SUM($B$160:$B$168)/9,0)</f>
-        <v>1012</v>
+        <f t="shared" ref="F161:F168" si="29">ROUND(B161+$C$159+$D$159*$F$6,0)+MAX(B161-$C$159,0)*2</f>
+        <v>3960</v>
       </c>
       <c r="G161" s="1">
         <v>0</v>
       </c>
       <c r="H161" s="16">
         <f t="shared" si="28"/>
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3870,14 +3877,14 @@
       </c>
       <c r="F162" s="1">
         <f t="shared" si="29"/>
-        <v>1012</v>
+        <v>3960</v>
       </c>
       <c r="G162" s="1">
         <v>2</v>
       </c>
       <c r="H162" s="16">
         <f t="shared" si="28"/>
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="163" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3889,14 +3896,14 @@
       </c>
       <c r="F163" s="1">
         <f t="shared" si="29"/>
-        <v>1052</v>
+        <v>4080</v>
       </c>
       <c r="G163" s="1">
         <v>6</v>
       </c>
       <c r="H163" s="16">
         <f t="shared" si="28"/>
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="164" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3908,14 +3915,14 @@
       </c>
       <c r="F164" s="1">
         <f t="shared" si="29"/>
-        <v>1092</v>
+        <v>4200</v>
       </c>
       <c r="G164" s="1">
         <v>6</v>
       </c>
       <c r="H164" s="16">
         <f t="shared" si="28"/>
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3927,14 +3934,14 @@
       </c>
       <c r="F165" s="1">
         <f t="shared" si="29"/>
-        <v>1092</v>
+        <v>4200</v>
       </c>
       <c r="G165" s="1">
         <v>11</v>
       </c>
       <c r="H165" s="16">
         <f t="shared" si="28"/>
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
     <row r="166" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3946,14 +3953,14 @@
       </c>
       <c r="F166" s="1">
         <f t="shared" si="29"/>
-        <v>1152</v>
+        <v>4380</v>
       </c>
       <c r="G166" s="1">
         <v>10</v>
       </c>
       <c r="H166" s="16">
         <f t="shared" si="28"/>
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="167" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3965,14 +3972,14 @@
       </c>
       <c r="F167" s="1">
         <f t="shared" si="29"/>
-        <v>1252</v>
+        <v>4680</v>
       </c>
       <c r="G167" s="1">
         <v>16</v>
       </c>
       <c r="H167" s="16">
         <f t="shared" si="28"/>
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="168" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3984,14 +3991,14 @@
       </c>
       <c r="F168" s="1">
         <f t="shared" si="29"/>
-        <v>1302</v>
+        <v>4830</v>
       </c>
       <c r="G168" s="1">
         <v>16</v>
       </c>
       <c r="H168" s="16">
         <f t="shared" si="28"/>
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new engines and changes to economy
</commit_message>
<xml_diff>
--- a/mode/LoneWolf/NewEngineFormulas.xlsx
+++ b/mode/LoneWolf/NewEngineFormulas.xlsx
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,7 +930,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="7">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F2" s="6">
         <v>0</v>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="H20" s="16">
         <f>ROUND(((F20-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1237,7 +1237,7 @@
       </c>
       <c r="H21" s="16">
         <f>ROUND(((F21-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="H22" s="16">
         <f>ROUND(((F22-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1275,7 +1275,7 @@
       </c>
       <c r="H23" s="16">
         <f>ROUND(((F23-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1311,7 +1311,7 @@
       </c>
       <c r="H25" s="16">
         <f t="shared" ref="H25:H32" si="1">ROUND(((F25-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="H26" s="16">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="H27" s="16">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1368,7 +1368,7 @@
       </c>
       <c r="H28" s="16">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1387,7 +1387,7 @@
       </c>
       <c r="H29" s="16">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="H30" s="16">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1425,7 +1425,7 @@
       </c>
       <c r="H31" s="16">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1444,7 +1444,7 @@
       </c>
       <c r="H32" s="16">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
       </c>
       <c r="H34" s="16">
         <f t="shared" ref="H34:H41" si="3">ROUND(((F34-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1499,7 +1499,7 @@
       </c>
       <c r="H35" s="16">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1518,7 +1518,7 @@
       </c>
       <c r="H36" s="16">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1537,7 +1537,7 @@
       </c>
       <c r="H37" s="16">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="H38" s="16">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1575,7 +1575,7 @@
       </c>
       <c r="H39" s="16">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1594,7 +1594,7 @@
       </c>
       <c r="H40" s="16">
         <f t="shared" si="3"/>
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="H41" s="16">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="H43" s="16">
         <f t="shared" ref="H43:H49" si="5">ROUND(((F43-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1668,7 +1668,7 @@
       </c>
       <c r="H44" s="16">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="45" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="H45" s="16">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="H46" s="16">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="H47" s="16">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="H48" s="16">
         <f t="shared" si="5"/>
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="H49" s="16">
         <f t="shared" si="5"/>
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1799,7 +1799,7 @@
       </c>
       <c r="H51" s="16">
         <f t="shared" ref="H51:H57" si="7">ROUND(((F51-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1818,7 +1818,7 @@
       </c>
       <c r="H52" s="16">
         <f t="shared" si="7"/>
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="H53" s="16">
         <f t="shared" si="7"/>
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="H54" s="16">
         <f t="shared" si="7"/>
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1875,7 +1875,7 @@
       </c>
       <c r="H55" s="16">
         <f t="shared" si="7"/>
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
       </c>
       <c r="H56" s="16">
         <f t="shared" si="7"/>
-        <v>37</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="H57" s="16">
         <f t="shared" si="7"/>
-        <v>44</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="H59" s="16">
         <f t="shared" ref="H59:H65" si="9">ROUND(((F59-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="H60" s="16">
         <f t="shared" si="9"/>
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1987,7 +1987,7 @@
       </c>
       <c r="H61" s="16">
         <f t="shared" si="9"/>
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="H62" s="16">
         <f t="shared" si="9"/>
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2025,7 +2025,7 @@
       </c>
       <c r="H63" s="16">
         <f t="shared" si="9"/>
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="64" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="H64" s="16">
         <f t="shared" si="9"/>
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="H65" s="16">
         <f t="shared" si="9"/>
-        <v>39</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2099,7 +2099,7 @@
       </c>
       <c r="H67" s="16">
         <f t="shared" ref="H67:H75" si="11">ROUND(((F67-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2118,7 +2118,7 @@
       </c>
       <c r="H68" s="16">
         <f t="shared" si="11"/>
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2137,7 +2137,7 @@
       </c>
       <c r="H69" s="16">
         <f t="shared" si="11"/>
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2156,7 +2156,7 @@
       </c>
       <c r="H70" s="16">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2175,7 +2175,7 @@
       </c>
       <c r="H71" s="16">
         <f t="shared" si="11"/>
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="72" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="H72" s="16">
         <f t="shared" si="11"/>
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="73" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="H73" s="16">
         <f t="shared" si="11"/>
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2232,7 +2232,7 @@
       </c>
       <c r="H74" s="16">
         <f t="shared" si="11"/>
-        <v>33</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="H75" s="16">
         <f t="shared" si="11"/>
-        <v>35</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -2287,7 +2287,7 @@
       </c>
       <c r="H77" s="16">
         <f t="shared" ref="H77:H83" si="13">ROUND(((F77-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>27</v>
+        <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="H78" s="16">
         <f t="shared" si="13"/>
-        <v>28</v>
+        <v>46</v>
       </c>
     </row>
     <row r="79" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2325,7 +2325,7 @@
       </c>
       <c r="H79" s="16">
         <f t="shared" si="13"/>
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2344,7 +2344,7 @@
       </c>
       <c r="H80" s="16">
         <f t="shared" si="13"/>
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="H81" s="16">
         <f t="shared" si="13"/>
-        <v>31</v>
+        <v>54</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2382,7 +2382,7 @@
       </c>
       <c r="H82" s="16">
         <f t="shared" si="13"/>
-        <v>34</v>
+        <v>61</v>
       </c>
     </row>
     <row r="83" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="H83" s="16">
         <f t="shared" si="13"/>
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -2437,7 +2437,7 @@
       </c>
       <c r="H85" s="16">
         <f>ROUND(((F85-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="86" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2456,7 +2456,7 @@
       </c>
       <c r="H86" s="16">
         <f>ROUND(((F86-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2475,7 +2475,7 @@
       </c>
       <c r="H87" s="16">
         <f>ROUND(((F87-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -2530,7 +2530,7 @@
       </c>
       <c r="H90" s="16">
         <f>ROUND(((F90-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="91" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="H91" s="16">
         <f>ROUND(((F91-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="H93" s="16">
         <f t="shared" ref="H93:H98" si="17">ROUND(((F93-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2604,7 +2604,7 @@
       </c>
       <c r="H94" s="16">
         <f t="shared" si="17"/>
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="95" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2623,7 +2623,7 @@
       </c>
       <c r="H95" s="16">
         <f t="shared" si="17"/>
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="96" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2642,7 +2642,7 @@
       </c>
       <c r="H96" s="16">
         <f t="shared" si="17"/>
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="97" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="H97" s="16">
         <f t="shared" si="17"/>
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="98" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2680,7 +2680,7 @@
       </c>
       <c r="H98" s="16">
         <f t="shared" si="17"/>
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="H100" s="16">
         <f t="shared" ref="H100:H111" si="19">ROUND(((F100-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="101" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2735,7 +2735,7 @@
       </c>
       <c r="H101" s="16">
         <f t="shared" si="19"/>
-        <v>32</v>
+        <v>57</v>
       </c>
     </row>
     <row r="102" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2754,7 +2754,7 @@
       </c>
       <c r="H102" s="16">
         <f t="shared" si="19"/>
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="103" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="H103" s="16">
         <f t="shared" si="19"/>
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="104" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2792,7 +2792,7 @@
       </c>
       <c r="H104" s="16">
         <f t="shared" si="19"/>
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="105" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2811,7 +2811,7 @@
       </c>
       <c r="H105" s="16">
         <f t="shared" si="19"/>
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="106" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="H106" s="16">
         <f t="shared" si="19"/>
-        <v>37</v>
+        <v>68</v>
       </c>
     </row>
     <row r="107" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2849,7 +2849,7 @@
       </c>
       <c r="H107" s="16">
         <f t="shared" si="19"/>
-        <v>37</v>
+        <v>68</v>
       </c>
     </row>
     <row r="108" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="H108" s="16">
         <f t="shared" si="19"/>
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="109" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2887,7 +2887,7 @@
       </c>
       <c r="H109" s="16">
         <f t="shared" si="19"/>
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="110" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2906,7 +2906,7 @@
       </c>
       <c r="H110" s="16">
         <f t="shared" si="19"/>
-        <v>44</v>
+        <v>84</v>
       </c>
     </row>
     <row r="111" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2925,7 +2925,7 @@
       </c>
       <c r="H111" s="16">
         <f t="shared" si="19"/>
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="H113" s="16">
         <f t="shared" ref="H113:H120" si="21">ROUND(((F113-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="114" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2980,7 +2980,7 @@
       </c>
       <c r="H114" s="16">
         <f t="shared" si="21"/>
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="115" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2999,7 +2999,7 @@
       </c>
       <c r="H115" s="16">
         <f t="shared" si="21"/>
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="116" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3018,7 +3018,7 @@
       </c>
       <c r="H116" s="16">
         <f t="shared" si="21"/>
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="117" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="H117" s="16">
         <f t="shared" si="21"/>
-        <v>39</v>
+        <v>73</v>
       </c>
     </row>
     <row r="118" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3056,7 +3056,7 @@
       </c>
       <c r="H118" s="16">
         <f t="shared" si="21"/>
-        <v>42</v>
+        <v>79</v>
       </c>
     </row>
     <row r="119" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3075,7 +3075,7 @@
       </c>
       <c r="H119" s="16">
         <f t="shared" si="21"/>
-        <v>45</v>
+        <v>87</v>
       </c>
     </row>
     <row r="120" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3094,7 +3094,7 @@
       </c>
       <c r="H120" s="16">
         <f t="shared" si="21"/>
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -3130,7 +3130,7 @@
       </c>
       <c r="H122" s="16">
         <f t="shared" ref="H122:H129" si="23">ROUND(((F122-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>32</v>
+        <v>55</v>
       </c>
     </row>
     <row r="123" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3149,7 +3149,7 @@
       </c>
       <c r="H123" s="16">
         <f t="shared" si="23"/>
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="124" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3168,7 +3168,7 @@
       </c>
       <c r="H124" s="16">
         <f t="shared" si="23"/>
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="125" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3187,7 +3187,7 @@
       </c>
       <c r="H125" s="16">
         <f t="shared" si="23"/>
-        <v>38</v>
+        <v>70</v>
       </c>
     </row>
     <row r="126" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="H126" s="16">
         <f t="shared" si="23"/>
-        <v>39</v>
+        <v>73</v>
       </c>
     </row>
     <row r="127" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3225,7 +3225,7 @@
       </c>
       <c r="H127" s="16">
         <f t="shared" si="23"/>
-        <v>42</v>
+        <v>79</v>
       </c>
     </row>
     <row r="128" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3244,7 +3244,7 @@
       </c>
       <c r="H128" s="16">
         <f t="shared" si="23"/>
-        <v>45</v>
+        <v>87</v>
       </c>
     </row>
     <row r="129" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="H129" s="16">
         <f t="shared" si="23"/>
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="H131" s="16">
         <f t="shared" ref="H131:H154" si="25">ROUND(((F131-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>31</v>
+        <v>55</v>
       </c>
     </row>
     <row r="132" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3318,7 +3318,7 @@
       </c>
       <c r="H132" s="16">
         <f t="shared" si="25"/>
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="133" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="H133" s="16">
         <f t="shared" si="25"/>
-        <v>32</v>
+        <v>57</v>
       </c>
     </row>
     <row r="134" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3356,7 +3356,7 @@
       </c>
       <c r="H134" s="16">
         <f t="shared" si="25"/>
-        <v>33</v>
+        <v>59</v>
       </c>
     </row>
     <row r="135" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3375,7 +3375,7 @@
       </c>
       <c r="H135" s="16">
         <f t="shared" si="25"/>
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="136" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3394,7 +3394,7 @@
       </c>
       <c r="H136" s="16">
         <f t="shared" si="25"/>
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="137" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="H137" s="16">
         <f t="shared" si="25"/>
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="138" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3432,7 +3432,7 @@
       </c>
       <c r="H138" s="16">
         <f t="shared" si="25"/>
-        <v>35</v>
+        <v>64</v>
       </c>
     </row>
     <row r="139" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3451,7 +3451,7 @@
       </c>
       <c r="H139" s="16">
         <f t="shared" si="25"/>
-        <v>36</v>
+        <v>65</v>
       </c>
     </row>
     <row r="140" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3470,7 +3470,7 @@
       </c>
       <c r="H140" s="16">
         <f t="shared" si="25"/>
-        <v>37</v>
+        <v>68</v>
       </c>
     </row>
     <row r="141" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3489,7 +3489,7 @@
       </c>
       <c r="H141" s="16">
         <f t="shared" si="25"/>
-        <v>37</v>
+        <v>68</v>
       </c>
     </row>
     <row r="142" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3508,7 +3508,7 @@
       </c>
       <c r="H142" s="16">
         <f t="shared" si="25"/>
-        <v>37</v>
+        <v>70</v>
       </c>
     </row>
     <row r="143" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3527,7 +3527,7 @@
       </c>
       <c r="H143" s="16">
         <f t="shared" si="25"/>
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="144" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3546,7 +3546,7 @@
       </c>
       <c r="H144" s="16">
         <f t="shared" si="25"/>
-        <v>39</v>
+        <v>73</v>
       </c>
     </row>
     <row r="145" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="H145" s="16">
         <f t="shared" si="25"/>
-        <v>41</v>
+        <v>78</v>
       </c>
     </row>
     <row r="146" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3584,7 +3584,7 @@
       </c>
       <c r="H146" s="16">
         <f t="shared" si="25"/>
-        <v>42</v>
+        <v>80</v>
       </c>
     </row>
     <row r="147" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3603,7 +3603,7 @@
       </c>
       <c r="H147" s="16">
         <f t="shared" si="25"/>
-        <v>44</v>
+        <v>84</v>
       </c>
     </row>
     <row r="148" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3622,7 +3622,7 @@
       </c>
       <c r="H148" s="16">
         <f t="shared" si="25"/>
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="149" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="H149" s="16">
         <f t="shared" si="25"/>
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="H151" s="16">
         <f t="shared" si="25"/>
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="152" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3696,7 +3696,7 @@
       </c>
       <c r="H152" s="16">
         <f t="shared" si="25"/>
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="153" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3715,7 +3715,7 @@
       </c>
       <c r="H153" s="16">
         <f t="shared" si="25"/>
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="154" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3734,7 +3734,7 @@
       </c>
       <c r="H154" s="16">
         <f t="shared" si="25"/>
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="155" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3753,7 +3753,7 @@
       </c>
       <c r="H155" s="16">
         <f>ROUND(((F155-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="156" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3772,7 +3772,7 @@
       </c>
       <c r="H156" s="16">
         <f>ROUND(((F156-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="157" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3791,7 +3791,7 @@
       </c>
       <c r="H157" s="16">
         <f>ROUND(((F157-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>48</v>
+        <v>94</v>
       </c>
     </row>
     <row r="158" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3810,7 +3810,7 @@
       </c>
       <c r="H158" s="16">
         <f>ROUND(((F158-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -3846,7 +3846,7 @@
       </c>
       <c r="H160" s="16">
         <f t="shared" ref="H160:H168" si="28">ROUND(((F160-$C$4)/($D$4-$C$4))*($D$2-$C$2),0)+$C$2</f>
-        <v>34</v>
+        <v>62</v>
       </c>
     </row>
     <row r="161" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="H161" s="16">
         <f t="shared" si="28"/>
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="162" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3884,7 +3884,7 @@
       </c>
       <c r="H162" s="16">
         <f t="shared" si="28"/>
-        <v>36</v>
+        <v>67</v>
       </c>
     </row>
     <row r="163" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3903,7 +3903,7 @@
       </c>
       <c r="H163" s="16">
         <f t="shared" si="28"/>
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="164" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3922,7 +3922,7 @@
       </c>
       <c r="H164" s="16">
         <f t="shared" si="28"/>
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="H165" s="16">
         <f t="shared" si="28"/>
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="166" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3960,7 +3960,7 @@
       </c>
       <c r="H166" s="16">
         <f t="shared" si="28"/>
-        <v>43</v>
+        <v>83</v>
       </c>
     </row>
     <row r="167" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3979,7 +3979,7 @@
       </c>
       <c r="H167" s="16">
         <f t="shared" si="28"/>
-        <v>48</v>
+        <v>94</v>
       </c>
     </row>
     <row r="168" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="H168" s="16">
         <f t="shared" si="28"/>
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>